<commit_message>
Update Data Karyawan Idea Imaji 2019.xlsx
</commit_message>
<xml_diff>
--- a/Data Karyawan Idea Imaji 2019.xlsx
+++ b/Data Karyawan Idea Imaji 2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C0CF78-99AB-466B-BE21-4914D035DBD7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E390384-9734-43EB-94A4-407E21811D0E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="0" windowWidth="20340" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Karyawan" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="315">
   <si>
     <t>`</t>
   </si>
@@ -1008,6 +1008,90 @@
   <si>
     <t>out 31 juli</t>
   </si>
+  <si>
+    <t>0042019</t>
+  </si>
+  <si>
+    <t>0052019</t>
+  </si>
+  <si>
+    <t>Yas Budaya</t>
+  </si>
+  <si>
+    <t>0062019</t>
+  </si>
+  <si>
+    <t>Gilang Permana</t>
+  </si>
+  <si>
+    <t>Jl. Bojongloa No.28 RT.03 RW.01 Kelurahan Panjunan Kecamatan Astana Anyar</t>
+  </si>
+  <si>
+    <t>Bandung, 23 November 1990</t>
+  </si>
+  <si>
+    <t>087722198848</t>
+  </si>
+  <si>
+    <t>3273102311900001</t>
+  </si>
+  <si>
+    <t>087823493007/Baria Sudarman (Ayah)</t>
+  </si>
+  <si>
+    <t>Videographer</t>
+  </si>
+  <si>
+    <t>yas@ideaimaji.com</t>
+  </si>
+  <si>
+    <t>Head of Creative</t>
+  </si>
+  <si>
+    <t>Jl. Mitra Dago Parahyangan Blok A No.12</t>
+  </si>
+  <si>
+    <t>Jl. Setra Dago Timur I No.10</t>
+  </si>
+  <si>
+    <t>Jakarta, 10 Desember 1980</t>
+  </si>
+  <si>
+    <t>08562193423</t>
+  </si>
+  <si>
+    <t>3273201012800001</t>
+  </si>
+  <si>
+    <t>081548728000/Fitri (Istri)</t>
+  </si>
+  <si>
+    <t>Fitri</t>
+  </si>
+  <si>
+    <t>Raha, 12 Juli 1983</t>
+  </si>
+  <si>
+    <t>Aldilas Akbar Satria</t>
+  </si>
+  <si>
+    <t>Sambek RT.02 RW.01 Wonosobo Jawa Tengah</t>
+  </si>
+  <si>
+    <t>Jl. Mutiara No.16 Turangga</t>
+  </si>
+  <si>
+    <t>Wonosobo, 9 Mei 1995</t>
+  </si>
+  <si>
+    <t>087710260645</t>
+  </si>
+  <si>
+    <t>3307090905950004</t>
+  </si>
+  <si>
+    <t>081321137005/Lukman (Teman)</t>
+  </si>
 </sst>
 </file>
 
@@ -1103,10 +1187,12 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1189,7 +1275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1212,20 +1298,7 @@
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1376,16 +1449,7 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1406,13 +1470,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1449,6 +1506,66 @@
     </xf>
     <xf numFmtId="12" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="12" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1774,7 +1891,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1819,9 +1936,9 @@
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="G1" s="76">
+      <c r="G1" s="68">
         <f ca="1">NOW()</f>
-        <v>43678.481474189815</v>
+        <v>43698.658742708336</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -1846,1551 +1963,1652 @@
       <c r="AC1" s="4"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="87" t="s">
+      <c r="F2" s="76" t="s">
         <v>234</v>
       </c>
-      <c r="G2" s="83" t="s">
+      <c r="G2" s="72" t="s">
         <v>283</v>
       </c>
-      <c r="H2" s="88" t="s">
+      <c r="H2" s="77" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="88" t="s">
+      <c r="I2" s="77" t="s">
         <v>182</v>
       </c>
-      <c r="J2" s="90" t="s">
+      <c r="J2" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="89" t="s">
+      <c r="K2" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="93" t="s">
+      <c r="L2" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="89" t="s">
+      <c r="M2" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="90" t="s">
+      <c r="O2" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17" t="s">
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="82"/>
-      <c r="X2" s="72"/>
-      <c r="Y2" s="81"/>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="81"/>
-      <c r="AC2" s="82"/>
-      <c r="AD2" s="73"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="71"/>
+      <c r="X2" s="64"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="65"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="15" t="s">
+      <c r="A3" s="75"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="86"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="16" t="s">
+      <c r="F3" s="75"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="86"/>
-      <c r="P3" s="17" t="s">
+      <c r="O3" s="75"/>
+      <c r="P3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="S3" s="18" t="s">
+      <c r="S3" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="T3" s="17" t="s">
+      <c r="T3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="U3" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="V3" s="18" t="s">
+      <c r="V3" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="W3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="X3" s="18" t="s">
+      <c r="X3" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="Y3" s="18" t="s">
+      <c r="Y3" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="Z3" s="17" t="s">
+      <c r="Z3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="AA3" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="AB3" s="18" t="s">
+      <c r="AB3" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="AC3" s="17" t="s">
+      <c r="AC3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AD3" s="17" t="s">
+      <c r="AD3" s="12" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="67">
+      <c r="F4" s="61">
         <v>39814</v>
       </c>
-      <c r="G4" s="24" t="str">
-        <f ca="1">DATEDIF(F4,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F4,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F4,$G$1,"MD")&amp;" Hri"</f>
-        <v>10 Th, 7 Bln, 0 Hri</v>
-      </c>
-      <c r="H4" s="25" t="s">
+      <c r="G4" s="19" t="str">
+        <f t="shared" ref="G4:G26" ca="1" si="0">DATEDIF(F4,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F4,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F4,$G$1,"MD")&amp;" Hri"</f>
+        <v>10 Th, 7 Bln, 20 Hri</v>
+      </c>
+      <c r="H4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="27">
+      <c r="L4" s="22">
         <v>3273202002820000</v>
       </c>
-      <c r="M4" s="28" t="s">
+      <c r="M4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="28"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="33" t="s">
+      <c r="N4" s="23"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="Q4" s="33" t="s">
+      <c r="Q4" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="33"/>
-      <c r="S4" s="60" t="s">
+      <c r="R4" s="28"/>
+      <c r="S4" s="55" t="s">
         <v>231</v>
       </c>
-      <c r="T4" s="33" t="s">
+      <c r="T4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33" t="s">
+      <c r="U4" s="28"/>
+      <c r="V4" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="W4" s="33" t="s">
+      <c r="W4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33" t="s">
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="Z4" s="33" t="s">
+      <c r="Z4" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="33"/>
-      <c r="AD4" s="39"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="34"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
+      <c r="A5" s="14">
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="25">
         <v>43344</v>
       </c>
-      <c r="G5" s="24" t="str">
-        <f ca="1">DATEDIF(F5,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F5,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F5,$G$1,"MD")&amp;" Hri"</f>
-        <v>0 Th, 11 Bln, 0 Hri</v>
-      </c>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 11 Bln, 20 Hri</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="60" t="s">
         <v>226</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L5" s="64" t="s">
+      <c r="L5" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="28"/>
-      <c r="O5" s="33" t="s">
+      <c r="N5" s="23"/>
+      <c r="O5" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="Q5" s="33" t="s">
+      <c r="Q5" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="33"/>
-      <c r="S5" s="24" t="s">
+      <c r="R5" s="28"/>
+      <c r="S5" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="T5" s="33" t="s">
+      <c r="T5" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="U5" s="33"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="39"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="39"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="34"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
-        <f t="shared" ref="A6:A23" si="0">A5+1</f>
+      <c r="A6" s="14">
+        <f t="shared" ref="A6:A25" si="1">A5+1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="62" t="s">
         <v>277</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="29">
         <v>41809</v>
       </c>
-      <c r="G6" s="24" t="str">
-        <f ca="1">DATEDIF(F6,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F6,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F6,$G$1,"MD")&amp;" Hri"</f>
-        <v>5 Th, 1 Bln, 13 Hri</v>
-      </c>
-      <c r="H6" s="35" t="s">
+      <c r="G6" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>5 Th, 2 Bln, 2 Hri</v>
+      </c>
+      <c r="H6" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="22">
         <v>3204085203860000</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="24" t="s">
+      <c r="O6" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24" t="s">
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="24" t="s">
+      <c r="T6" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="39"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="39"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="34"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="34"/>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="19">
-        <f t="shared" si="0"/>
+      <c r="A7" s="14">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="34">
+      <c r="F7" s="29">
         <v>42240</v>
       </c>
-      <c r="G7" s="24" t="str">
-        <f ca="1">DATEDIF(F7,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F7,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F7,$G$1,"MD")&amp;" Hri"</f>
-        <v>3 Th, 11 Bln, 8 Hri</v>
-      </c>
-      <c r="H7" s="35" t="s">
+      <c r="G7" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>3 Th, 11 Bln, 28 Hri</v>
+      </c>
+      <c r="H7" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="J7" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="38" t="s">
+      <c r="L7" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
-      <c r="Z7" s="24"/>
-      <c r="AA7" s="39"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="24"/>
-      <c r="AD7" s="39"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="19"/>
+      <c r="AC7" s="19"/>
+      <c r="AD7" s="34"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
-        <f t="shared" si="0"/>
+      <c r="A8" s="14">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F8" s="34">
+      <c r="F8" s="29">
         <v>42278</v>
       </c>
-      <c r="G8" s="24" t="str">
-        <f ca="1">DATEDIF(F8,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F8,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F8,$G$1,"MD")&amp;" Hri"</f>
-        <v>3 Th, 10 Bln, 0 Hri</v>
-      </c>
-      <c r="H8" s="35" t="s">
+      <c r="G8" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>3 Th, 10 Bln, 20 Hri</v>
+      </c>
+      <c r="H8" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="39"/>
-      <c r="M8" s="28" t="s">
+      <c r="L8" s="34"/>
+      <c r="M8" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="37" t="s">
+      <c r="N8" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="O8" s="24" t="s">
+      <c r="O8" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="Q8" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24" t="s">
+      <c r="R8" s="19"/>
+      <c r="S8" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="T8" s="24" t="s">
+      <c r="T8" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="39"/>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="24"/>
-      <c r="AD8" s="39"/>
-    </row>
-    <row r="9" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
-        <f t="shared" si="0"/>
+      <c r="U8" s="19"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="19"/>
+      <c r="X8" s="19"/>
+      <c r="Y8" s="19"/>
+      <c r="Z8" s="19"/>
+      <c r="AA8" s="34"/>
+      <c r="AB8" s="19"/>
+      <c r="AC8" s="19"/>
+      <c r="AD8" s="34"/>
+    </row>
+    <row r="9" spans="1:30" s="104" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="100">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="29">
         <v>42492</v>
       </c>
-      <c r="G9" s="24" t="str">
-        <f ca="1">DATEDIF(F9,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F9,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F9,$G$1,"MD")&amp;" Hri"</f>
-        <v>3 Th, 2 Bln, 30 Hri</v>
-      </c>
-      <c r="H9" s="35" t="s">
+      <c r="G9" s="18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>3 Th, 3 Bln, 19 Hri</v>
+      </c>
+      <c r="H9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="M9" s="41" t="s">
+      <c r="M9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="42" t="s">
+      <c r="N9" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="O9" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="39"/>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="24"/>
-      <c r="AD9" s="39"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="103"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="103"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
-        <f t="shared" si="0"/>
+      <c r="A10" s="14">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F10" s="29">
         <v>42590</v>
       </c>
-      <c r="G10" s="24" t="str">
-        <f ca="1">DATEDIF(F10,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F10,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F10,$G$1,"MD")&amp;" Hri"</f>
-        <v>2 Th, 11 Bln, 24 Hri</v>
-      </c>
-      <c r="H10" s="35" t="s">
+      <c r="G10" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>3 Th, 0 Bln, 13 Hri</v>
+      </c>
+      <c r="H10" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="I10" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="L10" s="27">
+      <c r="L10" s="22">
         <v>3204140601880000</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="M10" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="N10" s="42" t="s">
+      <c r="N10" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="O10" s="24" t="s">
+      <c r="O10" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="P10" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="Q10" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24" t="s">
+      <c r="R10" s="19"/>
+      <c r="S10" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="T10" s="24" t="s">
+      <c r="T10" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="24"/>
-      <c r="AD10" s="39"/>
+      <c r="U10" s="19"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="19"/>
+      <c r="Z10" s="19"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="19"/>
+      <c r="AC10" s="19"/>
+      <c r="AD10" s="34"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
-        <f t="shared" si="0"/>
+      <c r="A11" s="14">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="40">
         <v>43110</v>
       </c>
-      <c r="G11" s="24" t="str">
-        <f ca="1">DATEDIF(F11,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F11,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F11,$G$1,"MD")&amp;" Hri"</f>
-        <v>1 Th, 6 Bln, 22 Hri</v>
-      </c>
-      <c r="H11" s="46" t="s">
+      <c r="G11" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1 Th, 7 Bln, 11 Hri</v>
+      </c>
+      <c r="H11" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="I11" s="46" t="s">
+      <c r="I11" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="K11" s="47" t="s">
+      <c r="K11" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="L11" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="M11" s="47" t="s">
+      <c r="M11" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="N11" s="46"/>
-      <c r="O11" s="24" t="s">
+      <c r="N11" s="41"/>
+      <c r="O11" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24" t="s">
+      <c r="R11" s="19"/>
+      <c r="S11" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="T11" s="24" t="s">
+      <c r="T11" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="39"/>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="24"/>
-      <c r="AD11" s="39"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="34"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="34"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
-        <f t="shared" si="0"/>
+      <c r="A12" s="14">
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="71" t="s">
+      <c r="E12" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="40">
         <v>43136</v>
       </c>
-      <c r="G12" s="24" t="str">
-        <f ca="1">DATEDIF(F12,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F12,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F12,$G$1,"MD")&amp;" Hri"</f>
-        <v>1 Th, 5 Bln, 27 Hri</v>
-      </c>
-      <c r="H12" s="46" t="s">
+      <c r="G12" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1 Th, 6 Bln, 16 Hri</v>
+      </c>
+      <c r="H12" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="I12" s="46" t="s">
+      <c r="I12" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="K12" s="47" t="s">
+      <c r="K12" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="L12" s="27">
+      <c r="L12" s="22">
         <v>3217114506920010</v>
       </c>
-      <c r="M12" s="47"/>
-      <c r="N12" s="48" t="s">
+      <c r="M12" s="42"/>
+      <c r="N12" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="O12" s="24" t="s">
+      <c r="O12" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
-      <c r="AA12" s="39"/>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="24"/>
-      <c r="AD12" s="39"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="19"/>
+      <c r="Z12" s="19"/>
+      <c r="AA12" s="34"/>
+      <c r="AB12" s="19"/>
+      <c r="AC12" s="19"/>
+      <c r="AD12" s="34"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
-        <f t="shared" si="0"/>
+      <c r="A13" s="14">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="F13" s="45">
+      <c r="F13" s="40">
         <v>43174</v>
       </c>
-      <c r="G13" s="24" t="str">
-        <f ca="1">DATEDIF(F13,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F13,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F13,$G$1,"MD")&amp;" Hri"</f>
-        <v>1 Th, 4 Bln, 17 Hri</v>
-      </c>
-      <c r="H13" s="46" t="s">
+      <c r="G13" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1 Th, 5 Bln, 6 Hri</v>
+      </c>
+      <c r="H13" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="I13" s="46" t="s">
+      <c r="I13" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="K13" s="50" t="s">
+      <c r="K13" s="45" t="s">
         <v>152</v>
       </c>
-      <c r="L13" s="27" t="s">
+      <c r="L13" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="M13" s="47" t="s">
+      <c r="M13" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="N13" s="51" t="s">
+      <c r="N13" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="O13" s="24" t="s">
+      <c r="O13" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="P13" s="24" t="s">
+      <c r="P13" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="Q13" s="24" t="s">
+      <c r="Q13" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24" t="s">
+      <c r="R13" s="19"/>
+      <c r="S13" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="T13" s="24" t="s">
+      <c r="T13" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="U13" s="24"/>
-      <c r="V13" s="24" t="s">
+      <c r="U13" s="19"/>
+      <c r="V13" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="W13" s="33" t="s">
+      <c r="W13" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="X13" s="33"/>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24"/>
-      <c r="AA13" s="39"/>
-      <c r="AB13" s="24"/>
-      <c r="AC13" s="24"/>
-      <c r="AD13" s="39"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="19"/>
+      <c r="Z13" s="19"/>
+      <c r="AA13" s="34"/>
+      <c r="AB13" s="19"/>
+      <c r="AC13" s="19"/>
+      <c r="AD13" s="34"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <f t="shared" si="0"/>
+      <c r="A14" s="14">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="47">
         <v>43243</v>
       </c>
-      <c r="G14" s="24" t="str">
-        <f ca="1">DATEDIF(F14,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F14,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F14,$G$1,"MD")&amp;" Hri"</f>
-        <v>1 Th, 2 Bln, 9 Hri</v>
-      </c>
-      <c r="H14" s="46" t="s">
+      <c r="G14" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1 Th, 2 Bln, 29 Hri</v>
+      </c>
+      <c r="H14" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="I14" s="46" t="s">
+      <c r="I14" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
-      <c r="AA14" s="39"/>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="24"/>
-      <c r="AD14" s="39"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="42"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="19"/>
+      <c r="AC14" s="19"/>
+      <c r="AD14" s="34"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <f t="shared" si="0"/>
+      <c r="A15" s="14">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="44" t="s">
         <v>171</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="49">
         <v>43271</v>
       </c>
-      <c r="G15" s="24" t="str">
-        <f ca="1">DATEDIF(F15,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F15,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F15,$G$1,"MD")&amp;" Hri"</f>
-        <v>1 Th, 1 Bln, 12 Hri</v>
-      </c>
-      <c r="H15" s="46" t="s">
+      <c r="G15" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1 Th, 2 Bln, 1 Hri</v>
+      </c>
+      <c r="H15" s="41" t="s">
         <v>173</v>
       </c>
-      <c r="I15" s="46" t="s">
+      <c r="I15" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="K15" s="47" t="s">
+      <c r="K15" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="L15" s="27">
+      <c r="L15" s="22">
         <v>3273020808930010</v>
       </c>
-      <c r="M15" s="47"/>
-      <c r="N15" s="33" t="s">
+      <c r="M15" s="42"/>
+      <c r="N15" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="O15" s="33" t="s">
+      <c r="O15" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
-      <c r="AA15" s="39"/>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="24"/>
-      <c r="AD15" s="39"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="19"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="34"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
-        <f t="shared" si="0"/>
+      <c r="A16" s="14">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="E16" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="54">
+      <c r="F16" s="49">
         <v>43272</v>
       </c>
-      <c r="G16" s="24" t="str">
-        <f ca="1">DATEDIF(F16,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F16,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F16,$G$1,"MD")&amp;" Hri"</f>
-        <v>1 Th, 1 Bln, 11 Hri</v>
-      </c>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>1 Th, 2 Bln, 0 Hri</v>
+      </c>
+      <c r="H16" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="I16" s="46" t="s">
+      <c r="I16" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="J16" s="33" t="s">
+      <c r="J16" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="K16" s="47" t="s">
+      <c r="K16" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="L16" s="27">
+      <c r="L16" s="22">
         <v>5203070508960000</v>
       </c>
-      <c r="M16" s="47"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33" t="s">
+      <c r="M16" s="42"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
-      <c r="AA16" s="39"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="24"/>
-      <c r="AD16" s="39"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="19"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="19"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="34"/>
+      <c r="AB16" s="19"/>
+      <c r="AC16" s="19"/>
+      <c r="AD16" s="34"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <f t="shared" si="0"/>
+      <c r="A17" s="14">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="51" t="s">
         <v>191</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="E17" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="49">
         <v>43343</v>
       </c>
-      <c r="G17" s="24" t="str">
-        <f ca="1">DATEDIF(F17,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F17,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F17,$G$1,"MD")&amp;" Hri"</f>
-        <v>0 Th, 11 Bln, 1 Hri</v>
-      </c>
-      <c r="H17" s="46" t="s">
+      <c r="G17" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 11 Bln, 21 Hri</v>
+      </c>
+      <c r="H17" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="I17" s="46" t="s">
+      <c r="I17" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="J17" s="33" t="s">
+      <c r="J17" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="K17" s="47" t="s">
+      <c r="K17" s="42" t="s">
         <v>195</v>
       </c>
-      <c r="L17" s="55" t="s">
+      <c r="L17" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="M17" s="55" t="s">
+      <c r="M17" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33" t="s">
+      <c r="N17" s="28"/>
+      <c r="O17" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
-      <c r="Z17" s="24"/>
-      <c r="AA17" s="39"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="24"/>
-      <c r="AD17" s="39"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="19"/>
+      <c r="Z17" s="19"/>
+      <c r="AA17" s="34"/>
+      <c r="AB17" s="19"/>
+      <c r="AC17" s="19"/>
+      <c r="AD17" s="34"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
-        <f t="shared" si="0"/>
+      <c r="A18" s="14">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="53" t="s">
         <v>198</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="44" t="s">
         <v>215</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="54">
+      <c r="E18" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="49">
         <v>43340</v>
       </c>
-      <c r="G18" s="24" t="str">
-        <f ca="1">DATEDIF(F18,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F18,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F18,$G$1,"MD")&amp;" Hri"</f>
-        <v>0 Th, 11 Bln, 4 Hri</v>
-      </c>
-      <c r="H18" s="60" t="s">
+      <c r="G18" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 11 Bln, 24 Hri</v>
+      </c>
+      <c r="H18" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="I18" s="60" t="s">
+      <c r="I18" s="55" t="s">
         <v>223</v>
       </c>
-      <c r="J18" s="33"/>
-      <c r="K18" s="47"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
-      <c r="Z18" s="24"/>
-      <c r="AA18" s="39"/>
-      <c r="AB18" s="24"/>
-      <c r="AC18" s="24"/>
-      <c r="AD18" s="39"/>
-    </row>
-    <row r="19" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <f t="shared" si="0"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="19"/>
+      <c r="Z18" s="19"/>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="19"/>
+      <c r="AC18" s="19"/>
+      <c r="AD18" s="34"/>
+    </row>
+    <row r="19" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="C19" s="56" t="s">
+      <c r="C19" s="51" t="s">
         <v>200</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="E19" s="55" t="s">
+      <c r="E19" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="77">
+      <c r="F19" s="69">
         <v>43437</v>
       </c>
-      <c r="G19" s="24" t="str">
-        <f ca="1">DATEDIF(F19,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F19,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F19,$G$1,"MD")&amp;" Hri"</f>
-        <v>0 Th, 7 Bln, 29 Hri</v>
-      </c>
-      <c r="H19" s="60" t="s">
+      <c r="G19" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 8 Bln, 18 Hri</v>
+      </c>
+      <c r="H19" s="55" t="s">
         <v>202</v>
       </c>
-      <c r="I19" s="60" t="s">
+      <c r="I19" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="J19" s="61">
+      <c r="J19" s="56">
         <v>33373</v>
       </c>
-      <c r="K19" s="55"/>
-      <c r="L19" s="55" t="s">
+      <c r="K19" s="50"/>
+      <c r="L19" s="50" t="s">
         <v>201</v>
       </c>
-      <c r="M19" s="55"/>
-      <c r="N19" s="62"/>
-      <c r="O19" s="63" t="s">
+      <c r="M19" s="50"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="58" t="s">
         <v>218</v>
       </c>
-      <c r="P19" s="60" t="s">
+      <c r="P19" s="55" t="s">
         <v>204</v>
       </c>
-      <c r="Q19" s="60"/>
-      <c r="R19" s="60"/>
-      <c r="S19" s="55"/>
-      <c r="T19" s="55"/>
-      <c r="U19" s="55"/>
-      <c r="V19" s="62"/>
-      <c r="W19" s="62"/>
-      <c r="X19" s="62"/>
-      <c r="Y19" s="62"/>
-      <c r="Z19" s="62"/>
-      <c r="AA19" s="62"/>
-      <c r="AB19" s="62"/>
-      <c r="AC19" s="62"/>
-      <c r="AD19" s="62"/>
-    </row>
-    <row r="20" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
-        <f t="shared" si="0"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="57"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
+      <c r="Y19" s="57"/>
+      <c r="Z19" s="57"/>
+      <c r="AA19" s="57"/>
+      <c r="AB19" s="57"/>
+      <c r="AC19" s="57"/>
+      <c r="AD19" s="57"/>
+    </row>
+    <row r="20" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="E20" s="55" t="s">
+      <c r="E20" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="F20" s="77">
+      <c r="F20" s="69">
         <v>43437</v>
       </c>
-      <c r="G20" s="24" t="str">
-        <f ca="1">DATEDIF(F20,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F20,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F20,$G$1,"MD")&amp;" Hri"</f>
-        <v>0 Th, 7 Bln, 29 Hri</v>
-      </c>
-      <c r="H20" s="60" t="s">
+      <c r="G20" s="19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 8 Bln, 18 Hri</v>
+      </c>
+      <c r="H20" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="I20" s="60" t="s">
+      <c r="I20" s="55" t="s">
         <v>210</v>
       </c>
-      <c r="J20" s="61">
+      <c r="J20" s="56">
         <v>34736</v>
       </c>
-      <c r="K20" s="55" t="s">
+      <c r="K20" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="L20" s="55" t="s">
+      <c r="L20" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="M20" s="55" t="s">
+      <c r="M20" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="N20" s="62"/>
-      <c r="O20" s="63" t="s">
+      <c r="N20" s="57"/>
+      <c r="O20" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="60"/>
-      <c r="R20" s="60"/>
-      <c r="S20" s="55"/>
-      <c r="T20" s="55"/>
-      <c r="U20" s="55"/>
-      <c r="V20" s="62"/>
-      <c r="W20" s="62"/>
-      <c r="X20" s="62"/>
-      <c r="Y20" s="62"/>
-      <c r="Z20" s="62"/>
-      <c r="AA20" s="62"/>
-      <c r="AB20" s="62"/>
-      <c r="AC20" s="62"/>
-      <c r="AD20" s="62"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
-        <f t="shared" si="0"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="57"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
+      <c r="Y20" s="57"/>
+      <c r="Z20" s="57"/>
+      <c r="AA20" s="57"/>
+      <c r="AB20" s="57"/>
+      <c r="AC20" s="57"/>
+      <c r="AD20" s="57"/>
+    </row>
+    <row r="21" spans="1:30" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="83">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="84" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="79" t="s">
+      <c r="C21" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="86" t="s">
         <v>237</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="87" t="s">
         <v>238</v>
       </c>
-      <c r="F21" s="67">
+      <c r="F21" s="88">
         <v>43480</v>
       </c>
-      <c r="G21" s="24" t="str">
-        <f ca="1">DATEDIF(F21,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F21,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F21,$G$1,"MD")&amp;" Hri"</f>
-        <v>0 Th, 6 Bln, 17 Hri</v>
-      </c>
-      <c r="H21" s="46" t="s">
+      <c r="G21" s="87" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 7 Bln, 6 Hri</v>
+      </c>
+      <c r="H21" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="I21" s="46" t="s">
+      <c r="I21" s="51" t="s">
         <v>240</v>
       </c>
-      <c r="J21" s="33" t="s">
+      <c r="J21" s="87" t="s">
         <v>241</v>
       </c>
-      <c r="K21" s="47" t="s">
+      <c r="K21" s="89" t="s">
         <v>242</v>
       </c>
-      <c r="L21" s="64" t="s">
+      <c r="L21" s="90" t="s">
         <v>243</v>
       </c>
-      <c r="M21" s="47" t="s">
+      <c r="M21" s="89" t="s">
         <v>244</v>
       </c>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33" t="s">
+      <c r="N21" s="87"/>
+      <c r="O21" s="87" t="s">
         <v>245</v>
       </c>
-      <c r="P21" s="24" t="s">
+      <c r="P21" s="87" t="s">
         <v>246</v>
       </c>
-      <c r="Q21" s="33" t="s">
+      <c r="Q21" s="87" t="s">
         <v>166</v>
       </c>
-      <c r="R21" s="33" t="s">
+      <c r="R21" s="87" t="s">
         <v>250</v>
       </c>
-      <c r="S21" s="24" t="s">
+      <c r="S21" s="87" t="s">
         <v>247</v>
       </c>
-      <c r="T21" s="33" t="s">
+      <c r="T21" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="U21" s="33" t="s">
+      <c r="U21" s="87" t="s">
         <v>251</v>
       </c>
-      <c r="V21" s="24" t="s">
+      <c r="V21" s="87" t="s">
         <v>248</v>
       </c>
-      <c r="W21" s="33" t="s">
+      <c r="W21" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="X21" s="33" t="s">
+      <c r="X21" s="87" t="s">
         <v>252</v>
       </c>
-      <c r="Y21" s="24" t="s">
+      <c r="Y21" s="87" t="s">
         <v>253</v>
       </c>
-      <c r="Z21" s="33" t="s">
+      <c r="Z21" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="AA21" s="39" t="s">
+      <c r="AA21" s="91" t="s">
         <v>254</v>
       </c>
-      <c r="AB21" s="24" t="s">
+      <c r="AB21" s="87" t="s">
         <v>256</v>
       </c>
-      <c r="AC21" s="33" t="s">
+      <c r="AC21" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="AD21" s="39" t="s">
+      <c r="AD21" s="91" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
-        <f t="shared" si="0"/>
+    <row r="22" spans="1:30" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="83">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="93" t="s">
         <v>258</v>
       </c>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="85" t="s">
         <v>259</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="86" t="s">
         <v>260</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="87" t="s">
         <v>261</v>
       </c>
-      <c r="F22" s="67">
+      <c r="F22" s="88">
         <v>43514</v>
       </c>
-      <c r="G22" s="24" t="str">
-        <f ca="1">DATEDIF(F22,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F22,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F22,$G$1,"MD")&amp;" Hri"</f>
-        <v>0 Th, 5 Bln, 14 Hri</v>
-      </c>
-      <c r="H22" s="63" t="s">
+      <c r="G22" s="87" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 6 Bln, 3 Hri</v>
+      </c>
+      <c r="H22" s="51" t="s">
         <v>262</v>
       </c>
-      <c r="I22" s="68" t="s">
+      <c r="I22" s="94" t="s">
         <v>263</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="J22" s="87" t="s">
         <v>264</v>
       </c>
-      <c r="K22" s="69" t="s">
+      <c r="K22" s="89" t="s">
         <v>265</v>
       </c>
-      <c r="L22" s="27">
+      <c r="L22" s="95">
         <v>3273205005860010</v>
       </c>
-      <c r="M22" s="66" t="s">
+      <c r="M22" s="96" t="s">
         <v>266</v>
       </c>
-      <c r="N22" s="33" t="s">
+      <c r="N22" s="87" t="s">
         <v>267</v>
       </c>
-      <c r="O22" s="33" t="s">
+      <c r="O22" s="87" t="s">
         <v>268</v>
       </c>
-      <c r="P22" s="33" t="s">
+      <c r="P22" s="87" t="s">
         <v>269</v>
       </c>
-      <c r="Q22" s="33" t="s">
+      <c r="Q22" s="87" t="s">
         <v>139</v>
       </c>
-      <c r="R22" s="33" t="s">
+      <c r="R22" s="87" t="s">
         <v>270</v>
       </c>
-      <c r="S22" s="33" t="s">
+      <c r="S22" s="87" t="s">
         <v>271</v>
       </c>
-      <c r="T22" s="33" t="s">
+      <c r="T22" s="87" t="s">
         <v>110</v>
       </c>
-      <c r="U22" s="33" t="s">
+      <c r="U22" s="87" t="s">
         <v>272</v>
       </c>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="24"/>
-      <c r="AA22" s="39"/>
-      <c r="AB22" s="24"/>
-      <c r="AC22" s="24"/>
-      <c r="AD22" s="39"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
-        <f t="shared" si="0"/>
+      <c r="V22" s="87"/>
+      <c r="W22" s="87"/>
+      <c r="X22" s="87"/>
+      <c r="Y22" s="87"/>
+      <c r="Z22" s="87"/>
+      <c r="AA22" s="91"/>
+      <c r="AB22" s="87"/>
+      <c r="AC22" s="87"/>
+      <c r="AD22" s="91"/>
+    </row>
+    <row r="23" spans="1:30" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="83">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="93" t="s">
         <v>273</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="85" t="s">
         <v>274</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="86" t="s">
         <v>275</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="87" t="s">
         <v>276</v>
       </c>
-      <c r="F23" s="67">
+      <c r="F23" s="88">
         <v>43535</v>
       </c>
-      <c r="G23" s="24" t="str">
-        <f ca="1">DATEDIF(F23,$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F23,$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F23,$G$1,"MD")&amp;" Hri"</f>
-        <v>0 Th, 4 Bln, 21 Hri</v>
-      </c>
-      <c r="H23" s="63" t="s">
+      <c r="G23" s="87" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 5 Bln, 10 Hri</v>
+      </c>
+      <c r="H23" s="51" t="s">
         <v>278</v>
       </c>
-      <c r="I23" s="68" t="s">
+      <c r="I23" s="94" t="s">
         <v>279</v>
       </c>
-      <c r="J23" s="33" t="s">
+      <c r="J23" s="87" t="s">
         <v>280</v>
       </c>
-      <c r="K23" s="69" t="s">
+      <c r="K23" s="89" t="s">
         <v>281</v>
       </c>
-      <c r="L23" s="27">
+      <c r="L23" s="95">
         <v>3275096703970000</v>
       </c>
-      <c r="M23" s="47"/>
-      <c r="N23" s="33" t="s">
+      <c r="M23" s="89"/>
+      <c r="N23" s="87" t="s">
         <v>282</v>
       </c>
-      <c r="O23" s="33" t="s">
+      <c r="O23" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
-      <c r="Z23" s="24"/>
-      <c r="AA23" s="39"/>
-      <c r="AB23" s="24"/>
-      <c r="AC23" s="24"/>
-      <c r="AD23" s="39"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
-      <c r="Z24" s="4"/>
-      <c r="AB24" s="4"/>
-      <c r="AC24" s="4"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
-      <c r="T26" s="4"/>
-      <c r="U26" s="4"/>
-      <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-      <c r="Y26" s="4"/>
-      <c r="Z26" s="4"/>
-      <c r="AB26" s="4"/>
-      <c r="AC26" s="4"/>
+      <c r="P23" s="87"/>
+      <c r="Q23" s="87"/>
+      <c r="R23" s="87"/>
+      <c r="S23" s="87"/>
+      <c r="T23" s="87"/>
+      <c r="U23" s="87"/>
+      <c r="V23" s="87"/>
+      <c r="W23" s="87"/>
+      <c r="X23" s="87"/>
+      <c r="Y23" s="87"/>
+      <c r="Z23" s="87"/>
+      <c r="AA23" s="91"/>
+      <c r="AB23" s="87"/>
+      <c r="AC23" s="87"/>
+      <c r="AD23" s="91"/>
+    </row>
+    <row r="24" spans="1:30" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="83">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B24" s="84" t="s">
+        <v>287</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>308</v>
+      </c>
+      <c r="D24" s="86"/>
+      <c r="E24" s="87" t="s">
+        <v>297</v>
+      </c>
+      <c r="F24" s="88">
+        <v>43678</v>
+      </c>
+      <c r="G24" s="87" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 0 Bln, 20 Hri</v>
+      </c>
+      <c r="H24" s="94" t="s">
+        <v>309</v>
+      </c>
+      <c r="I24" s="51" t="s">
+        <v>310</v>
+      </c>
+      <c r="J24" s="87" t="s">
+        <v>311</v>
+      </c>
+      <c r="K24" s="97" t="s">
+        <v>312</v>
+      </c>
+      <c r="L24" s="90" t="s">
+        <v>313</v>
+      </c>
+      <c r="M24" s="89"/>
+      <c r="N24" s="98" t="s">
+        <v>314</v>
+      </c>
+      <c r="O24" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="P24" s="87"/>
+      <c r="Q24" s="87"/>
+      <c r="R24" s="87"/>
+      <c r="S24" s="87"/>
+      <c r="T24" s="87"/>
+      <c r="U24" s="87"/>
+      <c r="V24" s="87"/>
+      <c r="W24" s="87"/>
+      <c r="X24" s="87"/>
+      <c r="Y24" s="87"/>
+      <c r="Z24" s="87"/>
+      <c r="AA24" s="91"/>
+      <c r="AB24" s="87"/>
+      <c r="AC24" s="87"/>
+      <c r="AD24" s="91"/>
+    </row>
+    <row r="25" spans="1:30" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="83">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="84" t="s">
+        <v>288</v>
+      </c>
+      <c r="C25" s="85" t="s">
+        <v>289</v>
+      </c>
+      <c r="D25" s="86" t="s">
+        <v>298</v>
+      </c>
+      <c r="E25" s="87" t="s">
+        <v>299</v>
+      </c>
+      <c r="F25" s="88">
+        <v>43678</v>
+      </c>
+      <c r="G25" s="87" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 0 Bln, 20 Hri</v>
+      </c>
+      <c r="H25" s="51" t="s">
+        <v>300</v>
+      </c>
+      <c r="I25" s="51" t="s">
+        <v>301</v>
+      </c>
+      <c r="J25" s="87" t="s">
+        <v>302</v>
+      </c>
+      <c r="K25" s="97" t="s">
+        <v>303</v>
+      </c>
+      <c r="L25" s="90" t="s">
+        <v>304</v>
+      </c>
+      <c r="M25" s="89"/>
+      <c r="N25" s="98" t="s">
+        <v>305</v>
+      </c>
+      <c r="O25" s="87" t="s">
+        <v>218</v>
+      </c>
+      <c r="P25" s="87" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q25" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="R25" s="87" t="s">
+        <v>307</v>
+      </c>
+      <c r="S25" s="87"/>
+      <c r="T25" s="87"/>
+      <c r="U25" s="87"/>
+      <c r="V25" s="87"/>
+      <c r="W25" s="87"/>
+      <c r="X25" s="87"/>
+      <c r="Y25" s="87"/>
+      <c r="Z25" s="87"/>
+      <c r="AA25" s="91"/>
+      <c r="AB25" s="87"/>
+      <c r="AC25" s="87"/>
+      <c r="AD25" s="91"/>
+    </row>
+    <row r="26" spans="1:30" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="83">
+        <v>23</v>
+      </c>
+      <c r="B26" s="99" t="s">
+        <v>290</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87" t="s">
+        <v>214</v>
+      </c>
+      <c r="F26" s="88">
+        <v>43689</v>
+      </c>
+      <c r="G26" s="87" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>0 Th, 0 Bln, 9 Hri</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>292</v>
+      </c>
+      <c r="I26" s="51" t="s">
+        <v>203</v>
+      </c>
+      <c r="J26" s="87" t="s">
+        <v>293</v>
+      </c>
+      <c r="K26" s="97" t="s">
+        <v>294</v>
+      </c>
+      <c r="L26" s="90" t="s">
+        <v>295</v>
+      </c>
+      <c r="M26" s="89"/>
+      <c r="N26" s="98" t="s">
+        <v>296</v>
+      </c>
+      <c r="O26" s="87" t="s">
+        <v>91</v>
+      </c>
+      <c r="P26" s="87"/>
+      <c r="Q26" s="87"/>
+      <c r="R26" s="87"/>
+      <c r="S26" s="87"/>
+      <c r="T26" s="87"/>
+      <c r="U26" s="87"/>
+      <c r="V26" s="87"/>
+      <c r="W26" s="87"/>
+      <c r="X26" s="87"/>
+      <c r="Y26" s="87"/>
+      <c r="Z26" s="87"/>
+      <c r="AA26" s="91"/>
+      <c r="AB26" s="87"/>
+      <c r="AC26" s="87"/>
+      <c r="AD26" s="91"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
@@ -31116,10 +31334,11 @@
     <hyperlink ref="D21" r:id="rId7" xr:uid="{356E60E3-B099-4567-9E4C-8F4B2E1CEE83}"/>
     <hyperlink ref="D22" r:id="rId8" xr:uid="{3042EC6A-1BE8-4062-8944-15DC28E7360D}"/>
     <hyperlink ref="D23" r:id="rId9" xr:uid="{FDE84660-23AC-4A83-828B-947C43C93C68}"/>
+    <hyperlink ref="D25" r:id="rId10" xr:uid="{6742B525-7FD2-4549-A9F7-0FFC06DE72A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -31133,401 +31352,401 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A1" s="19">
+      <c r="A1" s="14">
         <f>'Data Karyawan'!A9+1</f>
         <v>7</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="62" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="75">
+      <c r="F1" s="67">
         <v>42583</v>
       </c>
-      <c r="G1" s="24" t="str">
+      <c r="G1" s="19" t="str">
         <f ca="1">DATEDIF(F1,'Data Karyawan'!$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F1,'Data Karyawan'!$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F1,'Data Karyawan'!$G$1,"MD")&amp;" Hri"</f>
-        <v>3 Th, 0 Bln, 0 Hri</v>
-      </c>
-      <c r="H1" s="35" t="s">
+        <v>3 Th, 0 Bln, 20 Hri</v>
+      </c>
+      <c r="H1" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="J1" s="31">
+      <c r="J1" s="26">
         <v>33772</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="27">
+      <c r="L1" s="22">
         <v>3216021706920010</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="42" t="s">
+      <c r="N1" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="24"/>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="39"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="34"/>
       <c r="AE1" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:31" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19">
+      <c r="A2" s="14">
         <f>OUT!A1+1</f>
         <v>8</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="71" t="s">
+      <c r="E2" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="34">
+      <c r="F2" s="29">
         <v>42583</v>
       </c>
-      <c r="G2" s="24" t="str">
+      <c r="G2" s="19" t="str">
         <f ca="1">DATEDIF(F2,'Data Karyawan'!$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F2,'Data Karyawan'!$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F2,'Data Karyawan'!$G$1,"MD")&amp;" Hri"</f>
-        <v>3 Th, 0 Bln, 0 Hri</v>
-      </c>
-      <c r="H2" s="74" t="s">
+        <v>3 Th, 0 Bln, 20 Hri</v>
+      </c>
+      <c r="H2" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="27">
+      <c r="L2" s="22">
         <v>3217024505950000</v>
       </c>
-      <c r="M2" s="41" t="s">
+      <c r="M2" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
-      <c r="Z2" s="24"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="24"/>
-      <c r="AC2" s="24"/>
-      <c r="AD2" s="39"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="34"/>
       <c r="AE2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19">
+    <row r="3" spans="1:31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
         <f>'Data Karyawan'!A11+1</f>
         <v>9</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="71" t="s">
+      <c r="E3" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="45">
+      <c r="F3" s="40">
         <v>43136</v>
       </c>
-      <c r="G3" s="24" t="str">
+      <c r="G3" s="19" t="str">
         <f ca="1">DATEDIF(F3,'Data Karyawan'!$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F3,'Data Karyawan'!$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F3,'Data Karyawan'!$G$1,"MD")&amp;" Hri"</f>
-        <v>1 Th, 5 Bln, 27 Hri</v>
-      </c>
-      <c r="H3" s="63" t="s">
+        <v>1 Th, 6 Bln, 16 Hri</v>
+      </c>
+      <c r="H3" s="58" t="s">
         <v>134</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="L3" s="27">
+      <c r="L3" s="22">
         <v>3211115107950010</v>
       </c>
-      <c r="M3" s="47"/>
-      <c r="N3" s="48" t="s">
+      <c r="M3" s="42"/>
+      <c r="N3" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="Q3" s="24" t="s">
+      <c r="Q3" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="24"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="24"/>
-      <c r="AD3" s="39"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="34"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="34"/>
       <c r="AE3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+    <row r="4" spans="1:31" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="14">
         <f>'Data Karyawan'!A10+1</f>
         <v>8</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="29">
         <v>42767</v>
       </c>
-      <c r="G4" s="24" t="str">
+      <c r="G4" s="19" t="str">
         <f ca="1">DATEDIF(F4,'Data Karyawan'!$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F4,'Data Karyawan'!$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F4,'Data Karyawan'!$G$1,"MD")&amp;" Hri"</f>
-        <v>2 Th, 6 Bln, 0 Hri</v>
-      </c>
-      <c r="H4" s="35" t="s">
+        <v>2 Th, 6 Bln, 20 Hri</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="31" t="s">
+      <c r="J4" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="L4" s="27" t="s">
+      <c r="L4" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="M4" s="41" t="s">
+      <c r="M4" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="N4" s="42" t="s">
+      <c r="N4" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="39"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="34"/>
       <c r="AE4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19">
+    <row r="5" spans="1:31" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A5" s="14">
         <f>'Data Karyawan'!A5+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="62" t="s">
         <v>167</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="29">
         <v>41799</v>
       </c>
-      <c r="G5" s="24" t="str">
+      <c r="G5" s="19" t="str">
         <f ca="1">DATEDIF(F5,'Data Karyawan'!$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F5,'Data Karyawan'!$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F5,'Data Karyawan'!$G$1,"MD")&amp;" Hri"</f>
-        <v>5 Th, 1 Bln, 23 Hri</v>
-      </c>
-      <c r="H5" s="74" t="s">
+        <v>5 Th, 2 Bln, 12 Hri</v>
+      </c>
+      <c r="H5" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="27">
+      <c r="L5" s="22">
         <v>637141701880009</v>
       </c>
-      <c r="M5" s="28" t="s">
+      <c r="M5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="O5" s="24" t="s">
+      <c r="O5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="Q5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24" t="s">
+      <c r="R5" s="19"/>
+      <c r="S5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="T5" s="24" t="s">
+      <c r="T5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="24"/>
-      <c r="AA5" s="39"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
-      <c r="AD5" s="39"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="34"/>
       <c r="AE5" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19">
+    <row r="6" spans="1:31" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
         <f>'Data Karyawan'!A14+1</f>
         <v>12</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="47">
         <v>43248</v>
       </c>
-      <c r="G6" s="24" t="str">
+      <c r="G6" s="19" t="str">
         <f ca="1">DATEDIF(F6,'Data Karyawan'!$G$1,"Y")&amp;" Th, "&amp;DATEDIF(F6,'Data Karyawan'!$G$1,"YM")&amp;" Bln, "&amp;DATEDIF(F6,'Data Karyawan'!$G$1,"MD")&amp;" Hri"</f>
-        <v>1 Th, 2 Bln, 4 Hri</v>
-      </c>
-      <c r="H6" s="60" t="s">
+        <v>1 Th, 2 Bln, 24 Hri</v>
+      </c>
+      <c r="H6" s="55" t="s">
         <v>224</v>
       </c>
-      <c r="I6" s="60" t="s">
+      <c r="I6" s="55" t="s">
         <v>203</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
-      <c r="Z6" s="24"/>
-      <c r="AA6" s="39"/>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="24"/>
-      <c r="AD6" s="39"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="19"/>
+      <c r="X6" s="19"/>
+      <c r="Y6" s="19"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="34"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="19"/>
+      <c r="AD6" s="34"/>
       <c r="AE6" t="s">
         <v>286</v>
       </c>

</xml_diff>